<commit_message>
Modify figure name for revised manuscript to eLife format.
</commit_message>
<xml_diff>
--- a/generation_time_Cp_removal/180925_generation_time_without_Cp.xlsx
+++ b/generation_time_Cp_removal/180925_generation_time_without_Cp.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuta_koganezawa/Documents/Wakamoto_lab/FpLrT10/New_MM/2nd_drug_exposure/Survivial_rate/before_Cp/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuta_koganezawa/Documents/Wakamoto_lab/paper_data/Phenotypic_Buffering/generation_time_Cp_removal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFCBF29-C0AE-3243-963B-5BFFFF27E99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E698DD-441E-3A41-910E-5CBE3C8D0495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15080" yWindow="460" windowWidth="10000" windowHeight="18540" xr2:uid="{6308C192-916F-1840-99FF-07306A350366}"/>
+    <workbookView xWindow="15080" yWindow="460" windowWidth="10000" windowHeight="18540" firstSheet="1" activeTab="2" xr2:uid="{6308C192-916F-1840-99FF-07306A350366}"/>
   </bookViews>
   <sheets>
-    <sheet name="dividing_cell" sheetId="1" r:id="rId1"/>
-    <sheet name="non-dividing_cell" sheetId="2" r:id="rId2"/>
-    <sheet name="resistant_cell" sheetId="3" r:id="rId3"/>
+    <sheet name="growth-restored cell lineage" sheetId="1" r:id="rId1"/>
+    <sheet name="growth-halted cell lineage" sheetId="2" r:id="rId2"/>
+    <sheet name="non-deleted cell lineage" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -447,7 +447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{306DE03C-C1A7-2D4D-9B3C-0C1BF7168EA1}">
   <dimension ref="A1:E184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+    <sheetView topLeftCell="A150" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E185" sqref="E185"/>
     </sheetView>
   </sheetViews>
@@ -10619,8 +10619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A631D5B-8B28-204A-8E46-685FECB9157E}">
   <dimension ref="A1:E530"/>
   <sheetViews>
-    <sheetView topLeftCell="A511" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E521" sqref="E521:E530"/>
+    <sheetView tabSelected="1" topLeftCell="A511" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E546" sqref="E546"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>

</xml_diff>